<commit_message>
uren registratie laatste fix & asset list update
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1151,7 +1151,7 @@
   <dimension ref="A1:N175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1263,11 +1263,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>6.583333333333333</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1525,7 +1525,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" s="48">
         <v>4</v>
@@ -1690,7 +1690,7 @@
       </c>
       <c r="D16" s="91">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="91">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Uren Registratie Inzet update
Uren registratie inzet
Scrumlog
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\FPS\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\GitHub\Gamelab 2.0\FPS\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,7 +530,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -862,6 +862,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1150,23 +1156,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" style="114" customWidth="1"/>
-    <col min="10" max="10" width="37.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" style="114" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="33" t="s">
         <v>6</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1313,7 +1319,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -1494,7 +1500,7 @@
       <c r="I9" s="93"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="73" t="s">
         <v>12</v>
       </c>
@@ -1516,27 +1522,27 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="79"/>
-      <c r="C11" s="47">
+      <c r="C11" s="131">
         <v>4</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="132">
         <v>2</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="132">
         <v>4</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="132">
         <v>4</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="132">
         <v>4</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="132">
         <v>3</v>
       </c>
       <c r="I11" s="49">
@@ -1545,7 +1551,7 @@
       <c r="J11" s="77"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>1</v>
       </c>
@@ -1578,7 +1584,7 @@
       </c>
       <c r="M12" s="119"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>2</v>
       </c>
@@ -1611,7 +1617,7 @@
       </c>
       <c r="M13" s="125"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>3</v>
       </c>
@@ -1644,7 +1650,7 @@
       </c>
       <c r="M14" s="126"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="75" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +1683,7 @@
       </c>
       <c r="M15" s="127"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
         <v>5</v>
       </c>
@@ -1719,7 +1725,7 @@
       </c>
       <c r="M16" s="128"/>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
@@ -1730,7 +1736,7 @@
       <c r="J17" s="13"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1745,7 +1751,7 @@
       <c r="J18" s="76"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1780,7 @@
       <c r="J19" s="77"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -1803,7 +1809,7 @@
       <c r="J20" s="77"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1832,7 +1838,7 @@
       <c r="J21" s="77"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1867,7 @@
       <c r="J22" s="77"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1890,7 +1896,7 @@
       <c r="J23" s="77"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1934,7 @@
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
       <c r="E25" s="93"/>
@@ -1937,7 +1943,7 @@
       <c r="H25" s="93"/>
       <c r="I25" s="93"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -1952,7 +1958,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -1981,7 +1987,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2010,7 +2016,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2039,7 +2045,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2068,7 +2074,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2103,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2135,7 +2141,7 @@
       <c r="J32" s="38"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="93"/>
       <c r="D33" s="93"/>
       <c r="E33" s="93"/>
@@ -2144,7 +2150,7 @@
       <c r="H33" s="93"/>
       <c r="I33" s="93"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2165,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2180,7 @@
       <c r="J35" s="18"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2195,7 @@
       <c r="J36" s="18"/>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>2</v>
       </c>
@@ -2206,7 +2212,7 @@
       <c r="J37" s="18"/>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>3</v>
       </c>
@@ -2221,7 +2227,7 @@
       <c r="J38" s="18"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2242,7 @@
       <c r="J39" s="20"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="93"/>
       <c r="D40" s="93"/>
       <c r="E40" s="93"/>
@@ -2245,7 +2251,7 @@
       <c r="H40" s="93"/>
       <c r="I40" s="93"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -2260,7 +2266,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2295,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>1</v>
       </c>
@@ -2318,7 +2324,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -2347,7 +2353,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
@@ -2376,7 +2382,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
@@ -2405,7 +2411,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>5</v>
       </c>
@@ -2443,7 +2449,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="93"/>
       <c r="D48" s="93"/>
       <c r="E48" s="93"/>
@@ -2452,7 +2458,7 @@
       <c r="H48" s="93"/>
       <c r="I48" s="93"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -2467,7 +2473,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2502,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
@@ -2525,7 +2531,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -2554,7 +2560,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
@@ -2583,7 +2589,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
@@ -2612,7 +2618,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2656,7 @@
       <c r="J55" s="43"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>
@@ -2659,7 +2665,7 @@
       <c r="H56" s="93"/>
       <c r="I56" s="93"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>18</v>
       </c>
@@ -2674,7 +2680,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="10"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
@@ -2703,7 +2709,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -2732,7 +2738,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2767,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
@@ -2790,7 +2796,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -2819,7 +2825,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2857,7 +2863,7 @@
       <c r="J63" s="43"/>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
       <c r="C64" s="109"/>
       <c r="D64" s="109"/>
@@ -2868,7 +2874,7 @@
       <c r="I64" s="109"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
@@ -2883,7 +2889,7 @@
       <c r="J65" s="23"/>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2918,7 @@
       <c r="J66" s="25"/>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +2947,7 @@
       <c r="J67" s="25"/>
       <c r="K67" s="10"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
@@ -2970,7 +2976,7 @@
       <c r="J68" s="25"/>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>3</v>
       </c>
@@ -2999,7 +3005,7 @@
       <c r="J69" s="25"/>
       <c r="K69" s="10"/>
     </row>
-    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>4</v>
       </c>
@@ -3028,7 +3034,7 @@
       <c r="J70" s="27"/>
       <c r="K70" s="10"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="38" t="s">
         <v>5</v>
       </c>
@@ -3066,7 +3072,7 @@
       <c r="J71" s="43"/>
       <c r="K71" s="10"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="93"/>
       <c r="D72" s="93"/>
       <c r="E72" s="93"/>
@@ -3075,7 +3081,7 @@
       <c r="H72" s="93"/>
       <c r="I72" s="93"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
@@ -3090,7 +3096,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>0</v>
       </c>
@@ -3119,7 +3125,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="10"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>1</v>
       </c>
@@ -3148,7 +3154,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="10"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>2</v>
       </c>
@@ -3177,7 +3183,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="10"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>3</v>
       </c>
@@ -3206,7 +3212,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="10"/>
     </row>
-    <row r="78" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>4</v>
       </c>
@@ -3235,7 +3241,7 @@
       <c r="J78" s="3"/>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>5</v>
       </c>
@@ -3273,7 +3279,7 @@
       <c r="J79" s="43"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="93"/>
       <c r="D80" s="93"/>
       <c r="E80" s="93"/>
@@ -3282,7 +3288,7 @@
       <c r="H80" s="93"/>
       <c r="I80" s="93"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3303,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3332,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>1</v>
       </c>
@@ -3355,7 +3361,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>2</v>
       </c>
@@ -3384,7 +3390,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>3</v>
       </c>
@@ -3413,7 +3419,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>4</v>
       </c>
@@ -3442,7 +3448,7 @@
       <c r="J86" s="3"/>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3486,7 @@
       <c r="J87" s="43"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="93"/>
       <c r="D88" s="93"/>
       <c r="E88" s="93"/>
@@ -3489,7 +3495,7 @@
       <c r="H88" s="93"/>
       <c r="I88" s="93"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>22</v>
       </c>
@@ -3504,7 +3510,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>0</v>
       </c>
@@ -3533,7 +3539,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>1</v>
       </c>
@@ -3562,7 +3568,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>2</v>
       </c>
@@ -3591,7 +3597,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
@@ -3620,7 +3626,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>4</v>
       </c>
@@ -3649,7 +3655,7 @@
       <c r="J94" s="3"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>5</v>
       </c>
@@ -3687,7 +3693,7 @@
       <c r="J95" s="43"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="93"/>
       <c r="D96" s="93"/>
       <c r="E96" s="93"/>
@@ -3696,7 +3702,7 @@
       <c r="H96" s="93"/>
       <c r="I96" s="93"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -3711,7 +3717,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>0</v>
       </c>
@@ -3740,7 +3746,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>1</v>
       </c>
@@ -3769,7 +3775,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>2</v>
       </c>
@@ -3798,7 +3804,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>3</v>
       </c>
@@ -3827,7 +3833,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>4</v>
       </c>
@@ -3856,7 +3862,7 @@
       <c r="J102" s="3"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>5</v>
       </c>
@@ -3894,7 +3900,7 @@
       <c r="J103" s="38"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C104" s="93"/>
       <c r="D104" s="93"/>
       <c r="E104" s="93"/>
@@ -3903,7 +3909,7 @@
       <c r="H104" s="93"/>
       <c r="I104" s="93"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
         <v>24</v>
       </c>
@@ -3918,7 +3924,7 @@
       <c r="J105" s="16"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>0</v>
       </c>
@@ -3933,7 +3939,7 @@
       <c r="J106" s="18"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>1</v>
       </c>
@@ -3948,7 +3954,7 @@
       <c r="J107" s="18"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="31" t="s">
         <v>2</v>
       </c>
@@ -3965,7 +3971,7 @@
       <c r="J108" s="18"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="31" t="s">
         <v>3</v>
       </c>
@@ -3980,7 +3986,7 @@
       <c r="J109" s="18"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="32" t="s">
         <v>4</v>
       </c>
@@ -3995,7 +4001,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="93"/>
       <c r="D111" s="93"/>
       <c r="E111" s="93"/>
@@ -4004,7 +4010,7 @@
       <c r="H111" s="93"/>
       <c r="I111" s="93"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>25</v>
       </c>
@@ -4019,7 +4025,7 @@
       <c r="J112" s="1"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>0</v>
       </c>
@@ -4048,7 +4054,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>1</v>
       </c>
@@ -4077,7 +4083,7 @@
       <c r="J114" s="2"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>2</v>
       </c>
@@ -4106,7 +4112,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>3</v>
       </c>
@@ -4135,7 +4141,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>4</v>
       </c>
@@ -4164,7 +4170,7 @@
       <c r="J117" s="3"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>5</v>
       </c>
@@ -4202,7 +4208,7 @@
       <c r="J118" s="38"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="93"/>
       <c r="D119" s="93"/>
       <c r="E119" s="93"/>
@@ -4211,7 +4217,7 @@
       <c r="H119" s="93"/>
       <c r="I119" s="93"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>26</v>
       </c>
@@ -4226,7 +4232,7 @@
       <c r="J120" s="1"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>0</v>
       </c>
@@ -4255,7 +4261,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>1</v>
       </c>
@@ -4284,7 +4290,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>2</v>
       </c>
@@ -4313,7 +4319,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>3</v>
       </c>
@@ -4342,7 +4348,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>4</v>
       </c>
@@ -4371,7 +4377,7 @@
       <c r="J125" s="3"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>5</v>
       </c>
@@ -4409,7 +4415,7 @@
       <c r="J126" s="38"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="93"/>
       <c r="D127" s="93"/>
       <c r="E127" s="93"/>
@@ -4418,7 +4424,7 @@
       <c r="H127" s="93"/>
       <c r="I127" s="93"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>27</v>
       </c>
@@ -4433,7 +4439,7 @@
       <c r="J128" s="1"/>
       <c r="K128" s="10"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>0</v>
       </c>
@@ -4462,7 +4468,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="10"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>1</v>
       </c>
@@ -4491,7 +4497,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="10"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>2</v>
       </c>
@@ -4520,7 +4526,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="10"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>3</v>
       </c>
@@ -4549,7 +4555,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="10"/>
     </row>
-    <row r="133" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>4</v>
       </c>
@@ -4578,7 +4584,7 @@
       <c r="J133" s="3"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>5</v>
       </c>
@@ -4616,7 +4622,7 @@
       <c r="J134" s="38"/>
       <c r="K134" s="10"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="93"/>
       <c r="D135" s="93"/>
       <c r="E135" s="93"/>
@@ -4625,7 +4631,7 @@
       <c r="H135" s="93"/>
       <c r="I135" s="93"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>28</v>
       </c>
@@ -4640,7 +4646,7 @@
       <c r="J136" s="23"/>
       <c r="K136" s="10"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>0</v>
       </c>
@@ -4669,7 +4675,7 @@
       <c r="J137" s="25"/>
       <c r="K137" s="10"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>1</v>
       </c>
@@ -4698,7 +4704,7 @@
       <c r="J138" s="25"/>
       <c r="K138" s="10"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>2</v>
       </c>
@@ -4727,7 +4733,7 @@
       <c r="J139" s="25"/>
       <c r="K139" s="10"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>3</v>
       </c>
@@ -4756,7 +4762,7 @@
       <c r="J140" s="25"/>
       <c r="K140" s="10"/>
     </row>
-    <row r="141" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>4</v>
       </c>
@@ -4785,7 +4791,7 @@
       <c r="J141" s="27"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>5</v>
       </c>
@@ -4823,7 +4829,7 @@
       <c r="J142" s="115"/>
       <c r="K142" s="10"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="93"/>
       <c r="D143" s="93"/>
@@ -4834,7 +4840,7 @@
       <c r="I143" s="93"/>
       <c r="J143" s="29"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>29</v>
       </c>
@@ -4849,7 +4855,7 @@
       <c r="J144" s="23"/>
       <c r="K144" s="10"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>0</v>
       </c>
@@ -4878,7 +4884,7 @@
       <c r="J145" s="25"/>
       <c r="K145" s="10"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>1</v>
       </c>
@@ -4907,7 +4913,7 @@
       <c r="J146" s="25"/>
       <c r="K146" s="10"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>2</v>
       </c>
@@ -4936,7 +4942,7 @@
       <c r="J147" s="25"/>
       <c r="K147" s="10"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>3</v>
       </c>
@@ -4965,7 +4971,7 @@
       <c r="J148" s="25"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>4</v>
       </c>
@@ -4994,7 +5000,7 @@
       <c r="J149" s="27"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5038,7 @@
       <c r="J150" s="38"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C151" s="93"/>
       <c r="D151" s="93"/>
       <c r="E151" s="93"/>
@@ -5041,7 +5047,7 @@
       <c r="H151" s="93"/>
       <c r="I151" s="93"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>30</v>
       </c>
@@ -5056,7 +5062,7 @@
       <c r="J152" s="1"/>
       <c r="K152" s="10"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>0</v>
       </c>
@@ -5085,7 +5091,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="10"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>1</v>
       </c>
@@ -5114,7 +5120,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="10"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>2</v>
       </c>
@@ -5143,7 +5149,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="10"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>3</v>
       </c>
@@ -5172,7 +5178,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="10"/>
     </row>
-    <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>4</v>
       </c>
@@ -5201,7 +5207,7 @@
       <c r="J157" s="3"/>
       <c r="K157" s="10"/>
     </row>
-    <row r="158" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>5</v>
       </c>
@@ -5239,7 +5245,7 @@
       <c r="J158" s="38"/>
       <c r="K158" s="10"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C159" s="93"/>
       <c r="D159" s="93"/>
       <c r="E159" s="93"/>
@@ -5248,7 +5254,7 @@
       <c r="H159" s="93"/>
       <c r="I159" s="93"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>31</v>
       </c>
@@ -5263,7 +5269,7 @@
       <c r="J160" s="1"/>
       <c r="K160" s="10"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>0</v>
       </c>
@@ -5292,7 +5298,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="10"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>1</v>
       </c>
@@ -5321,7 +5327,7 @@
       <c r="J162" s="2"/>
       <c r="K162" s="10"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>2</v>
       </c>
@@ -5350,7 +5356,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="10"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>3</v>
       </c>
@@ -5379,7 +5385,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="10"/>
     </row>
-    <row r="165" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>4</v>
       </c>
@@ -5408,7 +5414,7 @@
       <c r="J165" s="3"/>
       <c r="K165" s="10"/>
     </row>
-    <row r="166" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>5</v>
       </c>
@@ -5446,7 +5452,7 @@
       <c r="J166" s="38"/>
       <c r="K166" s="10"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C167" s="93"/>
       <c r="D167" s="93"/>
       <c r="E167" s="93"/>
@@ -5455,7 +5461,7 @@
       <c r="H167" s="93"/>
       <c r="I167" s="93"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>32</v>
       </c>
@@ -5470,7 +5476,7 @@
       <c r="J168" s="1"/>
       <c r="K168" s="10"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>0</v>
       </c>
@@ -5499,7 +5505,7 @@
       <c r="J169" s="2"/>
       <c r="K169" s="10"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>1</v>
       </c>
@@ -5528,7 +5534,7 @@
       <c r="J170" s="2"/>
       <c r="K170" s="10"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>2</v>
       </c>
@@ -5557,7 +5563,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="10"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>3</v>
       </c>
@@ -5586,7 +5592,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="10"/>
     </row>
-    <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>4</v>
       </c>
@@ -5615,7 +5621,7 @@
       <c r="J173" s="3"/>
       <c r="K173" s="10"/>
     </row>
-    <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>5</v>
       </c>
@@ -5653,7 +5659,7 @@
       <c r="J174" s="38"/>
       <c r="K174" s="10"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C175" s="93"/>
       <c r="D175" s="93"/>
       <c r="E175" s="93"/>

</xml_diff>

<commit_message>
Revert "Uren Registratie Inzet update"
This reverts commit 86e4dfc96ba256358fcea6361b04dfe17e9163a3.
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\GitHub\Gamelab 2.0\FPS\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\FPS\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,7 +530,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -862,12 +862,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1156,23 +1150,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
-    <col min="3" max="9" width="10.85546875" style="114" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
+    <col min="3" max="9" width="10.88671875" style="114" customWidth="1"/>
+    <col min="10" max="10" width="37.6640625" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="33" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1233,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1319,7 +1313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1393,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1435,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1484,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -1500,7 +1494,7 @@
       <c r="I9" s="93"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="73" t="s">
         <v>12</v>
       </c>
@@ -1522,27 +1516,27 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="79"/>
-      <c r="C11" s="131">
+      <c r="C11" s="47">
         <v>4</v>
       </c>
-      <c r="D11" s="132">
+      <c r="D11" s="48">
         <v>2</v>
       </c>
-      <c r="E11" s="132">
+      <c r="E11" s="48">
         <v>4</v>
       </c>
-      <c r="F11" s="132">
+      <c r="F11" s="48">
         <v>4</v>
       </c>
-      <c r="G11" s="132">
+      <c r="G11" s="48">
         <v>4</v>
       </c>
-      <c r="H11" s="132">
+      <c r="H11" s="48">
         <v>3</v>
       </c>
       <c r="I11" s="49">
@@ -1551,7 +1545,7 @@
       <c r="J11" s="77"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="74" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1578,7 @@
       </c>
       <c r="M12" s="119"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="74" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1611,7 @@
       </c>
       <c r="M13" s="125"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="74" t="s">
         <v>3</v>
       </c>
@@ -1650,7 +1644,7 @@
       </c>
       <c r="M14" s="126"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="75" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1677,7 @@
       </c>
       <c r="M15" s="127"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="75" t="s">
         <v>5</v>
       </c>
@@ -1725,7 +1719,7 @@
       </c>
       <c r="M16" s="128"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
@@ -1736,7 +1730,7 @@
       <c r="J17" s="13"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1751,7 +1745,7 @@
       <c r="J18" s="76"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1774,7 @@
       <c r="J19" s="77"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +1803,7 @@
       <c r="J20" s="77"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +1832,7 @@
       <c r="J21" s="77"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1861,7 @@
       <c r="J22" s="77"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1890,7 @@
       <c r="J23" s="77"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -1934,7 +1928,7 @@
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
       <c r="E25" s="93"/>
@@ -1943,7 +1937,7 @@
       <c r="H25" s="93"/>
       <c r="I25" s="93"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -1958,7 +1952,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -1987,7 +1981,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2016,7 +2010,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2045,7 +2039,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2074,7 +2068,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2103,7 +2097,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2141,7 +2135,7 @@
       <c r="J32" s="38"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="93"/>
       <c r="D33" s="93"/>
       <c r="E33" s="93"/>
@@ -2150,7 +2144,7 @@
       <c r="H33" s="93"/>
       <c r="I33" s="93"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>15</v>
       </c>
@@ -2165,7 +2159,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2174,7 @@
       <c r="J35" s="18"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>1</v>
       </c>
@@ -2195,7 +2189,7 @@
       <c r="J36" s="18"/>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>2</v>
       </c>
@@ -2212,7 +2206,7 @@
       <c r="J37" s="18"/>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2221,7 @@
       <c r="J38" s="18"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
         <v>4</v>
       </c>
@@ -2242,7 +2236,7 @@
       <c r="J39" s="20"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="93"/>
       <c r="D40" s="93"/>
       <c r="E40" s="93"/>
@@ -2251,7 +2245,7 @@
       <c r="H40" s="93"/>
       <c r="I40" s="93"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2260,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2289,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>1</v>
       </c>
@@ -2324,7 +2318,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -2353,7 +2347,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
@@ -2382,7 +2376,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
@@ -2411,7 +2405,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>5</v>
       </c>
@@ -2449,7 +2443,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C48" s="93"/>
       <c r="D48" s="93"/>
       <c r="E48" s="93"/>
@@ -2458,7 +2452,7 @@
       <c r="H48" s="93"/>
       <c r="I48" s="93"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -2473,7 +2467,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
@@ -2502,7 +2496,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
@@ -2531,7 +2525,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -2560,7 +2554,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2583,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
@@ -2618,7 +2612,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2650,7 @@
       <c r="J55" s="43"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>
@@ -2665,7 +2659,7 @@
       <c r="H56" s="93"/>
       <c r="I56" s="93"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>18</v>
       </c>
@@ -2680,7 +2674,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="10"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
@@ -2709,7 +2703,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -2738,7 +2732,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -2767,7 +2761,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
@@ -2796,7 +2790,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -2825,7 +2819,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2863,7 +2857,7 @@
       <c r="J63" s="43"/>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="10"/>
       <c r="C64" s="109"/>
       <c r="D64" s="109"/>
@@ -2874,7 +2868,7 @@
       <c r="I64" s="109"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
@@ -2889,7 +2883,7 @@
       <c r="J65" s="23"/>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
@@ -2918,7 +2912,7 @@
       <c r="J66" s="25"/>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>1</v>
       </c>
@@ -2947,7 +2941,7 @@
       <c r="J67" s="25"/>
       <c r="K67" s="10"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
@@ -2976,7 +2970,7 @@
       <c r="J68" s="25"/>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>3</v>
       </c>
@@ -3005,7 +2999,7 @@
       <c r="J69" s="25"/>
       <c r="K69" s="10"/>
     </row>
-    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>4</v>
       </c>
@@ -3034,7 +3028,7 @@
       <c r="J70" s="27"/>
       <c r="K70" s="10"/>
     </row>
-    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="38" t="s">
         <v>5</v>
       </c>
@@ -3072,7 +3066,7 @@
       <c r="J71" s="43"/>
       <c r="K71" s="10"/>
     </row>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C72" s="93"/>
       <c r="D72" s="93"/>
       <c r="E72" s="93"/>
@@ -3081,7 +3075,7 @@
       <c r="H72" s="93"/>
       <c r="I72" s="93"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
@@ -3096,7 +3090,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>0</v>
       </c>
@@ -3125,7 +3119,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="10"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>1</v>
       </c>
@@ -3154,7 +3148,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="10"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>2</v>
       </c>
@@ -3183,7 +3177,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="10"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>3</v>
       </c>
@@ -3212,7 +3206,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="10"/>
     </row>
-    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>4</v>
       </c>
@@ -3241,7 +3235,7 @@
       <c r="J78" s="3"/>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>5</v>
       </c>
@@ -3279,7 +3273,7 @@
       <c r="J79" s="43"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C80" s="93"/>
       <c r="D80" s="93"/>
       <c r="E80" s="93"/>
@@ -3288,7 +3282,7 @@
       <c r="H80" s="93"/>
       <c r="I80" s="93"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>21</v>
       </c>
@@ -3303,7 +3297,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3326,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>1</v>
       </c>
@@ -3361,7 +3355,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>2</v>
       </c>
@@ -3390,7 +3384,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>3</v>
       </c>
@@ -3419,7 +3413,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>4</v>
       </c>
@@ -3448,7 +3442,7 @@
       <c r="J86" s="3"/>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>5</v>
       </c>
@@ -3486,7 +3480,7 @@
       <c r="J87" s="43"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="93"/>
       <c r="D88" s="93"/>
       <c r="E88" s="93"/>
@@ -3495,7 +3489,7 @@
       <c r="H88" s="93"/>
       <c r="I88" s="93"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>22</v>
       </c>
@@ -3510,7 +3504,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3533,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>1</v>
       </c>
@@ -3568,7 +3562,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>2</v>
       </c>
@@ -3597,7 +3591,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
@@ -3626,7 +3620,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
         <v>4</v>
       </c>
@@ -3655,7 +3649,7 @@
       <c r="J94" s="3"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>5</v>
       </c>
@@ -3693,7 +3687,7 @@
       <c r="J95" s="43"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C96" s="93"/>
       <c r="D96" s="93"/>
       <c r="E96" s="93"/>
@@ -3702,7 +3696,7 @@
       <c r="H96" s="93"/>
       <c r="I96" s="93"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -3717,7 +3711,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>0</v>
       </c>
@@ -3746,7 +3740,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>1</v>
       </c>
@@ -3775,7 +3769,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>2</v>
       </c>
@@ -3804,7 +3798,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>3</v>
       </c>
@@ -3833,7 +3827,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>4</v>
       </c>
@@ -3862,7 +3856,7 @@
       <c r="J102" s="3"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>5</v>
       </c>
@@ -3900,7 +3894,7 @@
       <c r="J103" s="38"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C104" s="93"/>
       <c r="D104" s="93"/>
       <c r="E104" s="93"/>
@@ -3909,7 +3903,7 @@
       <c r="H104" s="93"/>
       <c r="I104" s="93"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="30" t="s">
         <v>24</v>
       </c>
@@ -3924,7 +3918,7 @@
       <c r="J105" s="16"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="31" t="s">
         <v>0</v>
       </c>
@@ -3939,7 +3933,7 @@
       <c r="J106" s="18"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="31" t="s">
         <v>1</v>
       </c>
@@ -3954,7 +3948,7 @@
       <c r="J107" s="18"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="31" t="s">
         <v>2</v>
       </c>
@@ -3971,7 +3965,7 @@
       <c r="J108" s="18"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="31" t="s">
         <v>3</v>
       </c>
@@ -3986,7 +3980,7 @@
       <c r="J109" s="18"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="32" t="s">
         <v>4</v>
       </c>
@@ -4001,7 +3995,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C111" s="93"/>
       <c r="D111" s="93"/>
       <c r="E111" s="93"/>
@@ -4010,7 +4004,7 @@
       <c r="H111" s="93"/>
       <c r="I111" s="93"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>25</v>
       </c>
@@ -4025,7 +4019,7 @@
       <c r="J112" s="1"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>0</v>
       </c>
@@ -4054,7 +4048,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>1</v>
       </c>
@@ -4083,7 +4077,7 @@
       <c r="J114" s="2"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>2</v>
       </c>
@@ -4112,7 +4106,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>3</v>
       </c>
@@ -4141,7 +4135,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>4</v>
       </c>
@@ -4170,7 +4164,7 @@
       <c r="J117" s="3"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>5</v>
       </c>
@@ -4208,7 +4202,7 @@
       <c r="J118" s="38"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C119" s="93"/>
       <c r="D119" s="93"/>
       <c r="E119" s="93"/>
@@ -4217,7 +4211,7 @@
       <c r="H119" s="93"/>
       <c r="I119" s="93"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>26</v>
       </c>
@@ -4232,7 +4226,7 @@
       <c r="J120" s="1"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>0</v>
       </c>
@@ -4261,7 +4255,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>1</v>
       </c>
@@ -4290,7 +4284,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>2</v>
       </c>
@@ -4319,7 +4313,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>3</v>
       </c>
@@ -4348,7 +4342,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
         <v>4</v>
       </c>
@@ -4377,7 +4371,7 @@
       <c r="J125" s="3"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>5</v>
       </c>
@@ -4415,7 +4409,7 @@
       <c r="J126" s="38"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C127" s="93"/>
       <c r="D127" s="93"/>
       <c r="E127" s="93"/>
@@ -4424,7 +4418,7 @@
       <c r="H127" s="93"/>
       <c r="I127" s="93"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>27</v>
       </c>
@@ -4439,7 +4433,7 @@
       <c r="J128" s="1"/>
       <c r="K128" s="10"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>0</v>
       </c>
@@ -4468,7 +4462,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="10"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>1</v>
       </c>
@@ -4497,7 +4491,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="10"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>2</v>
       </c>
@@ -4526,7 +4520,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="10"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>3</v>
       </c>
@@ -4555,7 +4549,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="10"/>
     </row>
-    <row r="133" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
         <v>4</v>
       </c>
@@ -4584,7 +4578,7 @@
       <c r="J133" s="3"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>5</v>
       </c>
@@ -4622,7 +4616,7 @@
       <c r="J134" s="38"/>
       <c r="K134" s="10"/>
     </row>
-    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C135" s="93"/>
       <c r="D135" s="93"/>
       <c r="E135" s="93"/>
@@ -4631,7 +4625,7 @@
       <c r="H135" s="93"/>
       <c r="I135" s="93"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>28</v>
       </c>
@@ -4646,7 +4640,7 @@
       <c r="J136" s="23"/>
       <c r="K136" s="10"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>0</v>
       </c>
@@ -4675,7 +4669,7 @@
       <c r="J137" s="25"/>
       <c r="K137" s="10"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>1</v>
       </c>
@@ -4704,7 +4698,7 @@
       <c r="J138" s="25"/>
       <c r="K138" s="10"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>2</v>
       </c>
@@ -4733,7 +4727,7 @@
       <c r="J139" s="25"/>
       <c r="K139" s="10"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>3</v>
       </c>
@@ -4762,7 +4756,7 @@
       <c r="J140" s="25"/>
       <c r="K140" s="10"/>
     </row>
-    <row r="141" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>4</v>
       </c>
@@ -4791,7 +4785,7 @@
       <c r="J141" s="27"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
         <v>5</v>
       </c>
@@ -4829,7 +4823,7 @@
       <c r="J142" s="115"/>
       <c r="K142" s="10"/>
     </row>
-    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="93"/>
       <c r="D143" s="93"/>
@@ -4840,7 +4834,7 @@
       <c r="I143" s="93"/>
       <c r="J143" s="29"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>29</v>
       </c>
@@ -4855,7 +4849,7 @@
       <c r="J144" s="23"/>
       <c r="K144" s="10"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>0</v>
       </c>
@@ -4884,7 +4878,7 @@
       <c r="J145" s="25"/>
       <c r="K145" s="10"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>1</v>
       </c>
@@ -4913,7 +4907,7 @@
       <c r="J146" s="25"/>
       <c r="K146" s="10"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>2</v>
       </c>
@@ -4942,7 +4936,7 @@
       <c r="J147" s="25"/>
       <c r="K147" s="10"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>3</v>
       </c>
@@ -4971,7 +4965,7 @@
       <c r="J148" s="25"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>4</v>
       </c>
@@ -5000,7 +4994,7 @@
       <c r="J149" s="27"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
         <v>5</v>
       </c>
@@ -5038,7 +5032,7 @@
       <c r="J150" s="38"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C151" s="93"/>
       <c r="D151" s="93"/>
       <c r="E151" s="93"/>
@@ -5047,7 +5041,7 @@
       <c r="H151" s="93"/>
       <c r="I151" s="93"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>30</v>
       </c>
@@ -5062,7 +5056,7 @@
       <c r="J152" s="1"/>
       <c r="K152" s="10"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>0</v>
       </c>
@@ -5091,7 +5085,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="10"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>1</v>
       </c>
@@ -5120,7 +5114,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="10"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>2</v>
       </c>
@@ -5149,7 +5143,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="10"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>3</v>
       </c>
@@ -5178,7 +5172,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="10"/>
     </row>
-    <row r="157" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
         <v>4</v>
       </c>
@@ -5207,7 +5201,7 @@
       <c r="J157" s="3"/>
       <c r="K157" s="10"/>
     </row>
-    <row r="158" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="6" t="s">
         <v>5</v>
       </c>
@@ -5245,7 +5239,7 @@
       <c r="J158" s="38"/>
       <c r="K158" s="10"/>
     </row>
-    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C159" s="93"/>
       <c r="D159" s="93"/>
       <c r="E159" s="93"/>
@@ -5254,7 +5248,7 @@
       <c r="H159" s="93"/>
       <c r="I159" s="93"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>31</v>
       </c>
@@ -5269,7 +5263,7 @@
       <c r="J160" s="1"/>
       <c r="K160" s="10"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>0</v>
       </c>
@@ -5298,7 +5292,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="10"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>1</v>
       </c>
@@ -5327,7 +5321,7 @@
       <c r="J162" s="2"/>
       <c r="K162" s="10"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>2</v>
       </c>
@@ -5356,7 +5350,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="10"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>3</v>
       </c>
@@ -5385,7 +5379,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="10"/>
     </row>
-    <row r="165" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>4</v>
       </c>
@@ -5414,7 +5408,7 @@
       <c r="J165" s="3"/>
       <c r="K165" s="10"/>
     </row>
-    <row r="166" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="6" t="s">
         <v>5</v>
       </c>
@@ -5452,7 +5446,7 @@
       <c r="J166" s="38"/>
       <c r="K166" s="10"/>
     </row>
-    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C167" s="93"/>
       <c r="D167" s="93"/>
       <c r="E167" s="93"/>
@@ -5461,7 +5455,7 @@
       <c r="H167" s="93"/>
       <c r="I167" s="93"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>32</v>
       </c>
@@ -5476,7 +5470,7 @@
       <c r="J168" s="1"/>
       <c r="K168" s="10"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>0</v>
       </c>
@@ -5505,7 +5499,7 @@
       <c r="J169" s="2"/>
       <c r="K169" s="10"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>1</v>
       </c>
@@ -5534,7 +5528,7 @@
       <c r="J170" s="2"/>
       <c r="K170" s="10"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>2</v>
       </c>
@@ -5563,7 +5557,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="10"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>3</v>
       </c>
@@ -5592,7 +5586,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="10"/>
     </row>
-    <row r="173" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="6" t="s">
         <v>4</v>
       </c>
@@ -5621,7 +5615,7 @@
       <c r="J173" s="3"/>
       <c r="K173" s="10"/>
     </row>
-    <row r="174" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>5</v>
       </c>
@@ -5659,7 +5653,7 @@
       <c r="J174" s="38"/>
       <c r="K174" s="10"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C175" s="93"/>
       <c r="D175" s="93"/>
       <c r="E175" s="93"/>

</xml_diff>

<commit_message>
Gun NOW WITH DELEGATES + Urenregistratie met inzet
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -886,6 +886,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1175,7 +1181,7 @@
   <dimension ref="A1:N175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="H12" sqref="H12:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1686,22 +1692,22 @@
       <c r="C15" s="108">
         <v>0</v>
       </c>
-      <c r="D15" s="106">
+      <c r="D15" s="135">
         <v>8</v>
       </c>
-      <c r="E15" s="106">
+      <c r="E15" s="135">
         <v>8</v>
       </c>
-      <c r="F15" s="106">
+      <c r="F15" s="135">
         <v>4</v>
       </c>
-      <c r="G15" s="106">
+      <c r="G15" s="135">
         <v>8</v>
       </c>
       <c r="H15" s="106">
         <v>0</v>
       </c>
-      <c r="I15" s="107">
+      <c r="I15" s="136">
         <v>7</v>
       </c>
       <c r="J15" s="77" t="s">

</xml_diff>

<commit_message>
gun ai enemy stuff test
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -892,9 +892,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1183,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,7 +1801,7 @@
       <c r="E19" s="132">
         <v>4</v>
       </c>
-      <c r="F19" s="137">
+      <c r="F19" s="132">
         <v>4</v>
       </c>
       <c r="G19" s="132">

</xml_diff>

<commit_message>
GUN 3.0 FFS EN URENREGISTRATIE
WOLLAH
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="56">
   <si>
     <t>Maandag</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Sam Ziek, Rief thuissituatie</t>
+  </si>
+  <si>
+    <t>Sam Ziek, Rief thuissituatie, Michiel laptop</t>
+  </si>
+  <si>
+    <t>Marc Ziek</t>
   </si>
 </sst>
 </file>
@@ -1180,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1249,15 +1255,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.67441860465116277</v>
+        <v>0.7021276595744681</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1293,11 +1299,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.93023255813953487</v>
+        <v>0.93617021276595747</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1333,7 +1339,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
@@ -1373,11 +1379,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.90697674418604646</v>
+        <v>0.91489361702127658</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1419,7 +1425,7 @@
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>1</v>
+        <v>0.91489361702127658</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1461,7 +1467,7 @@
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.51162790697674421</v>
+        <v>0.46808510638297873</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1506,11 +1512,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.7441860465116279</v>
+        <v>0.76595744680851063</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1545,7 +1551,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.7674418604651159</v>
+        <v>5.702127659574467</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1813,7 +1819,9 @@
       <c r="I19" s="49">
         <v>0</v>
       </c>
-      <c r="J19" s="77"/>
+      <c r="J19" s="77" t="s">
+        <v>54</v>
+      </c>
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1821,17 +1829,17 @@
         <v>1</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="47">
-        <v>0</v>
-      </c>
-      <c r="D20" s="48">
-        <v>0</v>
-      </c>
-      <c r="E20" s="48">
-        <v>0</v>
-      </c>
-      <c r="F20" s="48">
-        <v>0</v>
+      <c r="C20" s="131">
+        <v>4</v>
+      </c>
+      <c r="D20" s="132">
+        <v>4</v>
+      </c>
+      <c r="E20" s="132">
+        <v>4</v>
+      </c>
+      <c r="F20" s="132">
+        <v>4</v>
       </c>
       <c r="G20" s="48">
         <v>0</v>
@@ -1839,10 +1847,12 @@
       <c r="H20" s="48">
         <v>0</v>
       </c>
-      <c r="I20" s="49">
-        <v>0</v>
-      </c>
-      <c r="J20" s="77"/>
+      <c r="I20" s="133">
+        <v>4</v>
+      </c>
+      <c r="J20" s="77" t="s">
+        <v>55</v>
+      </c>
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1937,23 +1947,23 @@
         <v>5</v>
       </c>
       <c r="B24" s="45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C24" s="90">
         <f t="shared" ref="C24:G24" si="2">SUM(C19:C23)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24" s="91">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E24" s="91">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F24" s="91">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G24" s="91">
         <f t="shared" si="2"/>
@@ -1965,7 +1975,7 @@
       </c>
       <c r="I24" s="91">
         <f>SUM(I19:I23)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>

</xml_diff>

<commit_message>
Gun 3.0  en urenregistratie
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinedine038\Documents\GitHub\GameLab2\FPS\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinedine038\Desktop\GameLab2\FPS\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="57">
   <si>
     <t>Maandag</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Marc Ziek</t>
+  </si>
+  <si>
+    <t>Rief, Marc ziek. Carlo en Michiel wat later</t>
   </si>
 </sst>
 </file>
@@ -1186,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,7 +1258,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
@@ -1263,7 +1266,7 @@
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.7021276595744681</v>
+        <v>0.62264150943396224</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1299,11 +1302,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.93617021276595747</v>
+        <v>0.94339622641509435</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1339,7 +1342,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
@@ -1379,11 +1382,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.91489361702127658</v>
+        <v>0.90566037735849059</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1425,7 +1428,7 @@
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.91489361702127658</v>
+        <v>0.81132075471698117</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1463,11 +1466,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.46808510638297873</v>
+        <v>0.52830188679245282</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1512,11 +1515,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.76595744680851063</v>
+        <v>0.77358490566037741</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1551,7 +1554,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.702127659574467</v>
+        <v>5.584905660377359</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1863,25 +1866,27 @@
       <c r="C21" s="47">
         <v>0</v>
       </c>
-      <c r="D21" s="48">
-        <v>0</v>
-      </c>
-      <c r="E21" s="48">
-        <v>0</v>
-      </c>
-      <c r="F21" s="48">
-        <v>0</v>
+      <c r="D21" s="132">
+        <v>6</v>
+      </c>
+      <c r="E21" s="132">
+        <v>6</v>
+      </c>
+      <c r="F21" s="132">
+        <v>5</v>
       </c>
       <c r="G21" s="48">
         <v>0</v>
       </c>
-      <c r="H21" s="48">
-        <v>0</v>
-      </c>
-      <c r="I21" s="49">
-        <v>0</v>
-      </c>
-      <c r="J21" s="77"/>
+      <c r="H21" s="132">
+        <v>6</v>
+      </c>
+      <c r="I21" s="133">
+        <v>5</v>
+      </c>
+      <c r="J21" s="77" t="s">
+        <v>56</v>
+      </c>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1947,7 +1952,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="45">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C24" s="90">
         <f t="shared" ref="C24:G24" si="2">SUM(C19:C23)</f>
@@ -1955,15 +1960,15 @@
       </c>
       <c r="D24" s="91">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E24" s="91">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F24" s="91">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G24" s="91">
         <f t="shared" si="2"/>
@@ -1971,11 +1976,11 @@
       </c>
       <c r="H24" s="91">
         <f>SUM(H19:H23)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I24" s="91">
         <f>SUM(I19:I23)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>

</xml_diff>

<commit_message>
Uren registratie vrijdag en vandaag
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinedine038\Desktop\GameLab2\FPS\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\FPS\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,15 +1261,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.61111111111111116</v>
+        <v>0.59677419354838712</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1305,11 +1305,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.94444444444444442</v>
+        <v>0.95161290322580649</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1345,7 +1345,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
@@ -1385,11 +1385,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.90740740740740744</v>
+        <v>0.91935483870967738</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1427,11 +1427,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.81481481481481477</v>
+        <v>0.83870967741935487</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1469,11 +1469,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.53703703703703709</v>
+        <v>0.59677419354838712</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1518,11 +1518,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.77777777777777779</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.5925925925925926</v>
+        <v>5.645161290322581</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1932,22 +1932,22 @@
         <v>0</v>
       </c>
       <c r="D23" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E23" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G23" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I23" s="107">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J23" s="77"/>
       <c r="K23" s="10"/>
@@ -1957,7 +1957,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="45">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C24" s="90">
         <f t="shared" ref="C24:G24" si="2">SUM(C19:C23)</f>
@@ -1965,27 +1965,27 @@
       </c>
       <c r="D24" s="91">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E24" s="91">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F24" s="91">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G24" s="91">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H24" s="91">
         <f>SUM(H19:H23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I24" s="91">
         <f>SUM(I19:I23)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>
@@ -2020,22 +2020,22 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D27" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E27" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F27" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H27" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I27" s="49">
         <v>0</v>
@@ -2164,31 +2164,31 @@
         <v>5</v>
       </c>
       <c r="B32" s="45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C32" s="90">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="91">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E32" s="91">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F32" s="91">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G32" s="91">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="91">
         <f>SUM(H27:H31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I32" s="91">
         <f>SUM(I27:I31)</f>

</xml_diff>

<commit_message>
Uren Registratie gister en vandaag
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,15 +1261,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.59677419354838712</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1305,11 +1305,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.95161290322580649</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1345,7 +1345,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
@@ -1385,11 +1385,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.91935483870967738</v>
+        <v>0.93055555555555558</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1427,11 +1427,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.83870967741935487</v>
+        <v>0.86111111111111116</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1469,11 +1469,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.59677419354838712</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1518,11 +1518,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.74193548387096775</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.645161290322581</v>
+        <v>5.8333333333333339</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2049,25 +2049,25 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D28" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E28" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F28" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H28" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I28" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="10"/>
@@ -2078,25 +2078,25 @@
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="47">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D29" s="48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E29" s="48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F29" s="48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G29" s="48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H29" s="48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I29" s="49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="10"/>
@@ -2164,35 +2164,35 @@
         <v>5</v>
       </c>
       <c r="B32" s="45">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C32" s="90">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D32" s="91">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E32" s="91">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F32" s="91">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G32" s="91">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H32" s="91">
         <f>SUM(H27:H31)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I32" s="91">
         <f>SUM(I27:I31)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J32" s="38"/>
       <c r="K32" s="10"/>

</xml_diff>

<commit_message>
UseScript en uren registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1225,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1294,15 +1294,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.625</v>
+        <v>0.63207547169811318</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1338,11 +1338,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.97115384615384615</v>
+        <v>0.97169811320754718</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1378,11 +1378,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
-        <v>0.96153846153846156</v>
+        <v>0.96226415094339623</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>44</v>
@@ -1418,11 +1418,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.95192307692307687</v>
+        <v>0.95283018867924529</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1460,11 +1460,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.90384615384615385</v>
+        <v>0.90566037735849059</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1502,11 +1502,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.75</v>
+        <v>0.75471698113207553</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1551,11 +1551,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.66346153846153844</v>
+        <v>0.660377358490566</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.8269230769230775</v>
+        <v>5.8396226415094334</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2655,25 +2655,25 @@
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D53" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E53" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G53" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H53" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I53" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="10"/>
@@ -2712,35 +2712,35 @@
         <v>5</v>
       </c>
       <c r="B55" s="45">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C55" s="90">
         <f t="shared" ref="C55:G55" si="5">SUM(C50:C54)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D55" s="91">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E55" s="91">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F55" s="91">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G55" s="91">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H55" s="91">
         <f>SUM(H50:H54)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I55" s="92">
         <f>SUM(I50:I54)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="43"/>
       <c r="K55" s="10"/>

</xml_diff>

<commit_message>
Vorige was asset list changes, nu uren registratie
MY BAD
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:N175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1294,15 +1294,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.61403508771929827</v>
+        <v>0.6271186440677966</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1338,11 +1338,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.98245614035087714</v>
+        <v>0.98305084745762716</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1378,11 +1378,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
-        <v>0.96491228070175439</v>
+        <v>0.96610169491525422</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>44</v>
@@ -1418,11 +1418,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.92105263157894735</v>
+        <v>0.92372881355932202</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1460,11 +1460,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.91228070175438591</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1502,11 +1502,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.77192982456140347</v>
+        <v>0.71186440677966101</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1551,11 +1551,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.64912280701754388</v>
+        <v>0.66101694915254239</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.8157894736842097</v>
+        <v>5.7881355932203391</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2790,7 +2790,7 @@
         <v>4</v>
       </c>
       <c r="H58" s="48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I58" s="49">
         <v>0</v>
@@ -2804,25 +2804,25 @@
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D59" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E59" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F59" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G59" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H59" s="48">
         <v>0</v>
       </c>
       <c r="I59" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="10"/>
@@ -2919,35 +2919,35 @@
         <v>5</v>
       </c>
       <c r="B63" s="45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C63" s="90">
         <f t="shared" ref="C63:G63" si="6">SUM(C58:C62)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H63" s="91">
         <f>SUM(H58:H62)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I63" s="92">
         <f>SUM(I58:I62)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J63" s="43"/>
       <c r="K63" s="10"/>

</xml_diff>